<commit_message>
CLean up code, add exploratory code for features
</commit_message>
<xml_diff>
--- a/tags_CSV/FandomGenreCWTagClustering.xlsx
+++ b/tags_CSV/FandomGenreCWTagClustering.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryant/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryant/Desktop/Udacity/DSND/DSND_Capstone/Capstone/tags_CSV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB58A29-DA53-2741-91F7-7FB8EBEB950B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA65DDF8-BD46-2F42-BA0B-870813A6460B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28060" yWindow="500" windowWidth="28040" windowHeight="21100" xr2:uid="{57028D35-E7C7-7340-BDB4-5AB3C44230FC}"/>
+    <workbookView xWindow="-28060" yWindow="500" windowWidth="28040" windowHeight="21100" activeTab="5" xr2:uid="{57028D35-E7C7-7340-BDB4-5AB3C44230FC}"/>
   </bookViews>
   <sheets>
     <sheet name="fandomTags" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7735" uniqueCount="3048">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7746" uniqueCount="3048">
   <si>
     <t>Austin &amp; Murry-O'Keefe Families - Madeleine L'Engle</t>
   </si>
@@ -9572,7 +9572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E2595F-2779-F546-B074-BB776BF78D21}">
   <dimension ref="A1:BM112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -14085,8 +14085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E35D205-BECC-1B44-8F12-CA33A518C548}">
   <dimension ref="A1:WQ96"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A96" sqref="A1:XFD96"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17642,10 +17642,10 @@
       <c r="F10" s="1" t="s">
         <v>943</v>
       </c>
+      <c r="G10" s="1" t="s">
+        <v>1856</v>
+      </c>
       <c r="H10" s="1" t="s">
-        <v>1856</v>
-      </c>
-      <c r="I10" s="1" t="s">
         <v>1857</v>
       </c>
     </row>
@@ -20568,7 +20568,7 @@
   <dimension ref="A1:AA91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A44" sqref="A1:XFD44"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21720,10 +21720,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60D01B5-AF19-954E-AF0B-C76954C42FE2}">
-  <dimension ref="A1:D96"/>
+  <dimension ref="A1:P107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21755,408 +21755,420 @@
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>2835</v>
-      </c>
+      <c r="A4" s="3"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>2743</v>
-      </c>
+      <c r="A5" s="3" t="s">
+        <v>2835</v>
+      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>2836</v>
-      </c>
-      <c r="B6" s="2"/>
+        <v>2743</v>
+      </c>
       <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>2837</v>
-      </c>
-      <c r="B7" s="1"/>
+      <c r="A7" s="3"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>2836</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>2837</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>2855</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>2856</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
-        <v>2857</v>
-      </c>
+      <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>2858</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>2856</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>2859</v>
+        <v>2857</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>2761</v>
-      </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="3" t="s">
+        <v>2858</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>2860</v>
-      </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="3" t="s">
+        <v>2859</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>2861</v>
-      </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="3"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
-        <v>2739</v>
-      </c>
+      <c r="A16" s="3" t="s">
+        <v>2761</v>
+      </c>
+      <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
-        <v>2740</v>
-      </c>
+      <c r="A17" s="3" t="s">
+        <v>2860</v>
+      </c>
+      <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="C18" s="3" t="s">
-        <v>2838</v>
-      </c>
+      <c r="A18" s="3" t="s">
+        <v>2861</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="C19" s="3" t="s">
-        <v>2854</v>
-      </c>
+      <c r="B19" s="3" t="s">
+        <v>2739</v>
+      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="C20" s="3" t="s">
-        <v>2853</v>
-      </c>
+      <c r="B20" s="3" t="s">
+        <v>2740</v>
+      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
-        <v>2852</v>
+        <v>2838</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
-        <v>2851</v>
-      </c>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="C23" s="3" t="s">
-        <v>2750</v>
-      </c>
-      <c r="D23" s="1"/>
+        <v>2854</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="3" t="s">
+        <v>2853</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D24" s="3" t="s">
+        <v>2852</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="C25" s="3" t="s">
+        <v>2851</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="C26" s="3" t="s">
+        <v>2750</v>
+      </c>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D27" s="3" t="s">
         <v>2751</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D25" s="3" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D28" s="3" t="s">
         <v>2752</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>2862</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>2863</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>2864</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>2865</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
-        <v>2850</v>
-      </c>
+      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
-        <v>2849</v>
-      </c>
+      <c r="A31" s="3"/>
+      <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
-        <v>2848</v>
-      </c>
+      <c r="A32" s="3" t="s">
+        <v>2863</v>
+      </c>
+      <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B33" s="3"/>
-      <c r="C33" s="3" t="s">
-        <v>2847</v>
-      </c>
+    <row r="33" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
-        <v>2846</v>
-      </c>
+    <row r="34" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>2864</v>
+      </c>
+      <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B35" s="3" t="s">
-        <v>2845</v>
-      </c>
+    <row r="35" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
-        <v>2843</v>
-      </c>
+    <row r="36" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>2865</v>
+      </c>
+      <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="G36" s="3" t="s">
+        <v>2865</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>2850</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>2849</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>2848</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>2847</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>2846</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>2845</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>2843</v>
+      </c>
+      <c r="O36" s="3" t="s">
+        <v>2842</v>
+      </c>
+      <c r="P36" s="3" t="s">
+        <v>2844</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>2842</v>
+        <v>2850</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="I37" s="1"/>
+      <c r="P37" s="3" t="s">
+        <v>2745</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>2844</v>
+        <v>2849</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>2745</v>
+        <v>2848</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>2841</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+      <c r="B40" s="3"/>
+      <c r="C40" s="3" t="s">
+        <v>2847</v>
+      </c>
       <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
-        <v>2840</v>
+        <v>2846</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
-        <v>2767</v>
-      </c>
-      <c r="C42" s="2"/>
+        <v>2845</v>
+      </c>
+      <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-    </row>
-    <row r="43" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>2755</v>
-      </c>
-      <c r="B43" s="1"/>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
+        <v>2843</v>
+      </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
-        <v>2868</v>
-      </c>
-      <c r="C44" s="2"/>
+        <v>2842</v>
+      </c>
+      <c r="C44" s="1"/>
       <c r="D44" s="1"/>
-    </row>
-    <row r="45" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>2866</v>
-      </c>
-      <c r="B45" s="2"/>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+      <c r="B45" s="3" t="s">
+        <v>2844</v>
+      </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-    </row>
-    <row r="46" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>2736</v>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>2737</v>
-      </c>
-      <c r="B47" s="2"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
+        <v>2745</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+      <c r="B47" s="3"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
-    </row>
-    <row r="48" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>2769</v>
+        <v>2841</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
     </row>
     <row r="49" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>2774</v>
-      </c>
-      <c r="B49" s="1"/>
+      <c r="A49" s="3"/>
+      <c r="B49" s="3" t="s">
+        <v>2840</v>
+      </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
     </row>
     <row r="50" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3" t="s">
-        <v>2738</v>
-      </c>
-      <c r="C50" s="1"/>
+        <v>2767</v>
+      </c>
+      <c r="C50" s="2"/>
       <c r="D50" s="1"/>
     </row>
     <row r="51" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>2748</v>
-      </c>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="2"/>
       <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3" t="s">
-        <v>2747</v>
-      </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
+      <c r="A52" s="3" t="s">
+        <v>2755</v>
+      </c>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
     </row>
     <row r="53" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="3" t="s">
-        <v>2753</v>
-      </c>
-      <c r="C53" s="1"/>
+        <v>2868</v>
+      </c>
+      <c r="C53" s="2"/>
       <c r="D53" s="1"/>
     </row>
     <row r="54" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
-      <c r="B54" s="3" t="s">
-        <v>2754</v>
-      </c>
-      <c r="C54" s="1"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="2"/>
       <c r="D54" s="1"/>
     </row>
     <row r="55" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3" t="s">
-        <v>2757</v>
-      </c>
+      <c r="A55" s="3" t="s">
+        <v>2866</v>
+      </c>
+      <c r="B55" s="2"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
     </row>
     <row r="56" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
-      <c r="B56" s="3" t="s">
-        <v>2758</v>
-      </c>
-      <c r="C56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="1"/>
       <c r="D56" s="1"/>
     </row>
     <row r="57" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>2759</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>2760</v>
-      </c>
+        <v>2736</v>
+      </c>
+      <c r="B57" s="2"/>
       <c r="C57" s="2"/>
-      <c r="D57" s="1"/>
+      <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>2762</v>
+        <v>2737</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="1"/>
@@ -22164,107 +22176,112 @@
     </row>
     <row r="59" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>2763</v>
-      </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+        <v>2769</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
       <c r="D59" s="1"/>
     </row>
     <row r="60" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>2764</v>
-      </c>
-      <c r="B60" s="2"/>
+        <v>2774</v>
+      </c>
+      <c r="B60" s="1"/>
       <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
     </row>
     <row r="61" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
-        <v>2749</v>
-      </c>
-      <c r="B61" s="1"/>
+      <c r="A61" s="3"/>
+      <c r="B61" s="3" t="s">
+        <v>2738</v>
+      </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
     </row>
     <row r="62" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>2790</v>
-      </c>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
+        <v>2748</v>
+      </c>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
       <c r="D62" s="1"/>
     </row>
     <row r="63" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>2791</v>
-      </c>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
+      <c r="A63" s="3"/>
+      <c r="B63" s="3" t="s">
+        <v>2747</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
     </row>
     <row r="64" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>2746</v>
-      </c>
-      <c r="B64" s="1"/>
+      <c r="A64" s="3"/>
+      <c r="B64" s="3" t="s">
+        <v>2753</v>
+      </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
     </row>
     <row r="65" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>2779</v>
-      </c>
-      <c r="B65" s="1"/>
+      <c r="A65" s="3"/>
+      <c r="B65" s="3" t="s">
+        <v>2754</v>
+      </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
     </row>
     <row r="66" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
-        <v>2768</v>
-      </c>
-      <c r="B66" s="1"/>
+      <c r="A66" s="3"/>
+      <c r="B66" s="3" t="s">
+        <v>2757</v>
+      </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
     </row>
     <row r="67" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
-        <v>2771</v>
-      </c>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
+      <c r="A67" s="3"/>
+      <c r="B67" s="3" t="s">
+        <v>2758</v>
+      </c>
+      <c r="C67" s="2"/>
       <c r="D67" s="1"/>
     </row>
     <row r="68" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>2772</v>
-      </c>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
+        <v>2759</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>2760</v>
+      </c>
+      <c r="C68" s="2"/>
       <c r="D68" s="1"/>
     </row>
     <row r="69" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>2773</v>
-      </c>
-      <c r="B69" s="1"/>
+        <v>2762</v>
+      </c>
+      <c r="B69" s="2"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
     </row>
     <row r="70" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>2867</v>
-      </c>
-      <c r="B70" s="1"/>
+        <v>2763</v>
+      </c>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="1"/>
     </row>
     <row r="71" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>2778</v>
-      </c>
-      <c r="B71" s="1"/>
+        <v>2764</v>
+      </c>
+      <c r="B71" s="2"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
     </row>
     <row r="72" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>2775</v>
+        <v>2749</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -22272,30 +22289,30 @@
     </row>
     <row r="73" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>2776</v>
-      </c>
-      <c r="B73" s="1"/>
+        <v>2790</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
       <c r="D73" s="1"/>
     </row>
     <row r="74" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>2777</v>
+        <v>2791</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
     </row>
     <row r="75" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>2780</v>
-      </c>
-      <c r="B75" s="2"/>
+        <v>2746</v>
+      </c>
+      <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
     </row>
     <row r="76" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>2781</v>
+        <v>2779</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -22303,7 +22320,7 @@
     </row>
     <row r="77" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>2782</v>
+        <v>2768</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -22311,7 +22328,7 @@
     </row>
     <row r="78" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>2783</v>
+        <v>2771</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -22319,7 +22336,7 @@
     </row>
     <row r="79" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>2784</v>
+        <v>2772</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -22327,22 +22344,21 @@
     </row>
     <row r="80" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>2785</v>
+        <v>2773</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
     </row>
     <row r="81" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>2787</v>
+        <v>2867</v>
       </c>
       <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
     </row>
     <row r="82" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>2765</v>
+        <v>2778</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -22350,7 +22366,7 @@
     </row>
     <row r="83" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>2800</v>
+        <v>2775</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -22358,39 +22374,38 @@
     </row>
     <row r="84" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>2786</v>
+        <v>2776</v>
       </c>
       <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
       <c r="D84" s="1"/>
     </row>
     <row r="85" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>2788</v>
-      </c>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
+        <v>2777</v>
+      </c>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
     </row>
     <row r="86" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>2789</v>
+        <v>2780</v>
       </c>
       <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
     </row>
     <row r="87" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>2792</v>
-      </c>
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
+        <v>2781</v>
+      </c>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
     </row>
     <row r="88" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>2793</v>
+        <v>2782</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -22398,7 +22413,7 @@
     </row>
     <row r="89" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>2794</v>
+        <v>2783</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -22406,7 +22421,7 @@
     </row>
     <row r="90" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>2796</v>
+        <v>2784</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -22414,15 +22429,14 @@
     </row>
     <row r="91" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>2798</v>
+        <v>2785</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
     </row>
     <row r="92" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>2802</v>
+        <v>2787</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -22430,7 +22444,7 @@
     </row>
     <row r="93" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>2799</v>
+        <v>2765</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -22438,7 +22452,7 @@
     </row>
     <row r="94" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -22446,7 +22460,7 @@
     </row>
     <row r="95" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>2803</v>
+        <v>2786</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -22454,10 +22468,98 @@
     </row>
     <row r="96" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
+        <v>2788</v>
+      </c>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+    </row>
+    <row r="97" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>2789</v>
+      </c>
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
+    </row>
+    <row r="98" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>2792</v>
+      </c>
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+    </row>
+    <row r="99" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>2793</v>
+      </c>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+    </row>
+    <row r="100" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>2794</v>
+      </c>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+    </row>
+    <row r="101" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>2796</v>
+      </c>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+    </row>
+    <row r="102" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>2798</v>
+      </c>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+    </row>
+    <row r="103" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>2802</v>
+      </c>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+    </row>
+    <row r="104" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>2799</v>
+      </c>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+    </row>
+    <row r="105" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>2801</v>
+      </c>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+    </row>
+    <row r="106" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>2803</v>
+      </c>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+    </row>
+    <row r="107" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
         <v>2804</v>
       </c>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22468,8 +22570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533B8ECD-8152-D043-959E-1A7668431CFE}">
   <dimension ref="A1:BJ154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>